<commit_message>
Atualização automática de SAO_JERONIMO.xlsx
</commit_message>
<xml_diff>
--- a/SAO_JERONIMO.xlsx
+++ b/SAO_JERONIMO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{36F695D0-3A08-44ED-B960-847FEF8D86A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E125BBA3-AFF1-4F3F-A7E6-3AC9BE008412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1201,7 +1201,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{AD263237-BD18-4231-AC6B-F5EBE6467E48}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{E7470218-1C8D-4829-8F17-974FE109EA24}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1231,10 +1231,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30489D50-CE3D-40E5-A90D-2A1740C792C3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7927E4F7-DFE0-485E-A10F-137391448BCF}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1272,7 +1272,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82E4E7DF-4B27-463F-AC85-CBCE64197741}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{146BF93E-2092-4626-96B3-CF4B29837168}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1335,7 +1335,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4EB63CD-9ADD-484B-9A06-62FAAC27C49D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F0627B9-28B6-4F73-B395-EC4B27023644}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1354,7 +1354,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A49A259-E2BC-4DC7-520F-712523CE03B4}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62ADA3F7-3F8C-C988-C6E5-A2D68F6D8732}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1403,7 +1403,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C559B7A1-A265-6BDF-2FE5-6AA7AB1DE921}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34A6877E-1712-0B03-2F65-6FB7DF379569}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1422,7 +1422,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E5234E2-ECED-DBE2-7B38-DC9A0CA943D9}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{152532D1-67E3-7D60-E6B8-236CEF869DB7}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1453,7 +1453,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D38E63B-E079-3C14-0E15-415EA0C8301B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68F428E4-9242-2714-9063-E3C7EEFA0E87}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1484,7 +1484,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EBBF68D1-2746-C41B-9B2B-A08C2A969214}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A24F67B1-C620-891D-5380-30DF508781AA}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1527,7 +1527,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A46B6207-E4E8-4783-8E73-745155F9372E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3552572B-696C-4244-81C1-97E1414495C8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1565,7 +1565,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B3B6066-866B-457D-BCFF-20116C221669}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62FE84CE-B0B7-42B6-A1A8-1F3C44389759}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1608,7 +1608,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99C44550-E1C2-4F6F-9447-3089DF9881C4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A90997E0-CD5C-4B3C-B13A-B828E095173F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1921,7 +1921,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF13DDE0-3741-4B50-AA04-A7E40C56F5A8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D340B226-B4C4-4087-9E67-0DAA2BE646A6}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>